<commit_message>
more work on projects
</commit_message>
<xml_diff>
--- a/public/assets/ProjectContent.xlsx
+++ b/public/assets/ProjectContent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Work\Personal Projects\MyWebsite\website\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50581DC-ED62-4358-91F8-622BA86DA5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C827C5D-2C6D-4E7E-915D-970962ACD75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43D118BB-33E5-473A-9FB5-B0D457F42264}"/>
   </bookViews>
@@ -1194,6 +1194,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1201,12 +1207,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1559,10 +1559,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19A312E-A7DF-4680-8C5B-375D2B52973A}">
   <dimension ref="A1:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="H29" sqref="H29"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.75" x14ac:dyDescent="0.2"/>
@@ -2525,7 +2525,7 @@
       <c r="AB21" s="62"/>
     </row>
     <row r="22" spans="1:28" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="91" t="s">
         <v>119</v>
       </c>
       <c r="B22" s="69" t="s">
@@ -2565,7 +2565,7 @@
       <c r="AA22" s="37"/>
     </row>
     <row r="23" spans="1:28" ht="132" x14ac:dyDescent="0.2">
-      <c r="A23" s="94"/>
+      <c r="A23" s="91"/>
       <c r="B23" s="69" t="s">
         <v>9</v>
       </c>
@@ -2605,7 +2605,7 @@
       <c r="AA23" s="37"/>
     </row>
     <row r="24" spans="1:28" ht="72" x14ac:dyDescent="0.2">
-      <c r="A24" s="94"/>
+      <c r="A24" s="91"/>
       <c r="B24" s="69" t="s">
         <v>10</v>
       </c>
@@ -2641,7 +2641,7 @@
       <c r="AA24" s="37"/>
     </row>
     <row r="25" spans="1:28" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="94"/>
+      <c r="A25" s="91"/>
       <c r="B25" s="69" t="s">
         <v>33</v>
       </c>
@@ -2679,7 +2679,7 @@
       <c r="AA25" s="37"/>
     </row>
     <row r="26" spans="1:28" ht="55.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="95"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="69" t="s">
         <v>40</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="AB27" s="62"/>
     </row>
     <row r="28" spans="1:28" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="91" t="s">
+      <c r="A28" s="93" t="s">
         <v>120</v>
       </c>
       <c r="B28" s="70" t="s">
@@ -2785,7 +2785,7 @@
       <c r="AA28" s="38"/>
     </row>
     <row r="29" spans="1:28" ht="171" x14ac:dyDescent="0.2">
-      <c r="A29" s="92"/>
+      <c r="A29" s="94"/>
       <c r="B29" s="70" t="s">
         <v>28</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="AA29" s="38"/>
     </row>
     <row r="30" spans="1:28" ht="156" x14ac:dyDescent="0.2">
-      <c r="A30" s="92"/>
+      <c r="A30" s="94"/>
       <c r="B30" s="70" t="s">
         <v>27</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="AA30" s="38"/>
     </row>
     <row r="31" spans="1:28" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="92"/>
+      <c r="A31" s="94"/>
       <c r="B31" s="70" t="s">
         <v>32</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="AA31" s="38"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
+      <c r="A32" s="95"/>
       <c r="B32" s="70"/>
       <c r="D32" s="20"/>
       <c r="F32" s="13"/>

</xml_diff>